<commit_message>
fix the vanishing point approach
- fix the vanishing point approach
- add option dialog
- add additional test photos
</commit_message>
<xml_diff>
--- a/parameter_estimation.xlsx
+++ b/parameter_estimation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>No.</t>
   </si>
@@ -54,6 +54,15 @@
   <si>
     <t>Min</t>
   </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>Aerial</t>
+  </si>
+  <si>
+    <t>Cylinder</t>
+  </si>
 </sst>
 </file>
 
@@ -76,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +95,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -117,12 +132,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,14 +447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -476,34 +501,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>-0.29819600000000002</v>
+        <v>0.21995000000000001</v>
       </c>
       <c r="C2" s="3">
-        <v>56.853000000000002</v>
+        <v>56.356099999999998</v>
       </c>
       <c r="D2" s="3">
-        <v>2.4041999999999999</v>
+        <v>1.6278999999999999</v>
       </c>
       <c r="E2" s="3">
-        <v>65.891000000000005</v>
+        <v>66.403700000000001</v>
       </c>
       <c r="F2" s="3">
-        <v>-3.4750000000000001</v>
+        <v>-3.6</v>
       </c>
       <c r="G2" s="3">
-        <v>-7.5374999999999996</v>
+        <v>-7.4625000000000004</v>
       </c>
       <c r="H2" s="3">
-        <v>38.576900000000002</v>
+        <v>38.201300000000003</v>
       </c>
       <c r="I2" s="3">
-        <v>8.5500000000000007</v>
+        <v>8.25</v>
       </c>
       <c r="J2" s="3">
-        <v>20.100000000000001</v>
+        <v>19.649999999999999</v>
       </c>
       <c r="K2" s="3">
-        <v>8</v>
+        <v>8.15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -996,7 +1021,7 @@
         <v>20.95</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1031,7 +1056,7 @@
         <v>18.95</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1066,7 +1091,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1101,7 +1126,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1136,7 +1161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1171,7 +1196,7 @@
         <v>30.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1206,7 +1231,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1241,7 +1266,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1276,7 +1301,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1311,7 +1336,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1346,22 +1371,45 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>13.6492</v>
+      </c>
+      <c r="C27" s="6">
+        <v>74.290199999999999</v>
+      </c>
+      <c r="D27" s="6">
+        <v>6.7292199999999998</v>
+      </c>
+      <c r="E27" s="6">
+        <v>31.331299999999999</v>
+      </c>
+      <c r="F27" s="6">
+        <v>-2.6</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="H27" s="6">
+        <v>89.145399999999995</v>
+      </c>
+      <c r="I27" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="J27" s="6">
+        <v>22.1</v>
+      </c>
+      <c r="K27" s="6">
+        <v>15.5</v>
+      </c>
+      <c r="L27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1396,7 +1444,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1431,7 +1479,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1466,7 +1514,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1501,7 +1549,7 @@
         <v>22.75</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1536,22 +1584,45 @@
         <v>39.85</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>38.5</v>
+      </c>
+      <c r="C33" s="6">
+        <v>27.143899999999999</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.659</v>
+      </c>
+      <c r="E33" s="6">
+        <v>57.2866</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="6">
+        <v>45.770899999999997</v>
+      </c>
+      <c r="I33" s="6">
+        <v>14.5</v>
+      </c>
+      <c r="J33" s="6">
+        <v>35.1</v>
+      </c>
+      <c r="K33" s="6">
+        <v>11.5</v>
+      </c>
+      <c r="L33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1586,22 +1657,42 @@
         <v>45.65</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>-4.4029699999999998</v>
+      </c>
+      <c r="C35" s="3">
+        <v>66.207999999999998</v>
+      </c>
+      <c r="D35" s="3">
+        <v>-0.56032000000000004</v>
+      </c>
+      <c r="E35" s="3">
+        <v>34.518099999999997</v>
+      </c>
+      <c r="F35" s="3">
+        <v>12.125</v>
+      </c>
+      <c r="G35" s="3">
+        <v>2.3624999999999998</v>
+      </c>
+      <c r="H35" s="3">
+        <v>80.468400000000003</v>
+      </c>
+      <c r="I35" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="J35" s="3">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="K35" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1636,111 +1727,716 @@
         <v>28.65</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="4">
-        <f>MAX(B2:B36)</f>
-        <v>-0.29819600000000002</v>
-      </c>
-      <c r="C38" s="4">
-        <f t="shared" ref="C38:K38" si="0">MAX(C2:C36)</f>
-        <v>70.976100000000002</v>
-      </c>
-      <c r="D38" s="4">
-        <f t="shared" si="0"/>
-        <v>11.7377</v>
-      </c>
-      <c r="E38" s="4">
-        <f t="shared" si="0"/>
-        <v>87.4529</v>
-      </c>
-      <c r="F38" s="4">
-        <f t="shared" si="0"/>
-        <v>12.137499999999999</v>
-      </c>
-      <c r="G38" s="4">
-        <f t="shared" si="0"/>
-        <v>13.824999999999999</v>
-      </c>
-      <c r="H38" s="4">
-        <f t="shared" si="0"/>
-        <v>136.988</v>
-      </c>
-      <c r="I38" s="4">
-        <f t="shared" si="0"/>
-        <v>48.6</v>
-      </c>
-      <c r="J38" s="4">
-        <f t="shared" si="0"/>
-        <v>44.05</v>
-      </c>
-      <c r="K38" s="4">
-        <f t="shared" si="0"/>
-        <v>45.65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3">
+        <v>-11.3726</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="3">
+        <v>-1.2146600000000001</v>
+      </c>
+      <c r="E37" s="3">
+        <v>26.9711</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2</v>
+      </c>
+      <c r="H37" s="3">
+        <v>104.248</v>
+      </c>
+      <c r="I37" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="J37" s="3">
+        <v>38.9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="L37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3">
+        <v>-27.985399999999998</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="3">
+        <v>13.81</v>
+      </c>
+      <c r="E38" s="3">
+        <v>51.640999999999998</v>
+      </c>
+      <c r="F38" s="3">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="G38" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="H38" s="3">
+        <v>51.6678</v>
+      </c>
+      <c r="I38" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="J38" s="3">
+        <v>24.65</v>
+      </c>
+      <c r="K38" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="L38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3">
+        <v>-1.8256399999999999</v>
+      </c>
+      <c r="C39" s="3">
+        <v>54.678899999999999</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.433143</v>
+      </c>
+      <c r="E39" s="3">
+        <v>58.015099999999997</v>
+      </c>
+      <c r="F39" s="3">
+        <v>-4.4249999999999998</v>
+      </c>
+      <c r="G39" s="3">
+        <v>-1.0375000000000001</v>
+      </c>
+      <c r="H39" s="3">
+        <v>45.087200000000003</v>
+      </c>
+      <c r="I39" s="3">
+        <v>23</v>
+      </c>
+      <c r="J39" s="3">
+        <v>7.05</v>
+      </c>
+      <c r="K39" s="3">
+        <v>41.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3">
+        <v>-6.7423599999999997</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.77398</v>
+      </c>
+      <c r="E40" s="3">
+        <v>43.235900000000001</v>
+      </c>
+      <c r="F40" s="3">
+        <v>-1.8625</v>
+      </c>
+      <c r="G40" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="H40" s="3">
+        <v>63.085099999999997</v>
+      </c>
+      <c r="I40" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="J40" s="3">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="K40" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3">
+        <v>3.8489</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45.489800000000002</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.30410199999999998</v>
+      </c>
+      <c r="E41" s="3">
+        <v>70.647000000000006</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <v>-3.8125</v>
+      </c>
+      <c r="H41" s="3">
+        <v>35.278100000000002</v>
+      </c>
+      <c r="I41" s="3">
+        <v>8.25</v>
+      </c>
+      <c r="J41" s="3">
+        <v>29.25</v>
+      </c>
+      <c r="K41" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3">
+        <v>-16.863499999999998</v>
+      </c>
+      <c r="C42" s="3">
+        <v>38.0092</v>
+      </c>
+      <c r="D42" s="3">
+        <v>2.6054400000000002</v>
+      </c>
+      <c r="E42" s="3">
+        <v>50.5657</v>
+      </c>
+      <c r="F42" s="3">
+        <v>-0.67500000000000004</v>
+      </c>
+      <c r="G42" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="H42" s="3">
+        <v>52.928899999999999</v>
+      </c>
+      <c r="I42" s="3">
+        <v>27.35</v>
+      </c>
+      <c r="J42" s="3">
+        <v>22.95</v>
+      </c>
+      <c r="K42" s="3">
+        <v>21.65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3">
+        <v>-16.2971</v>
+      </c>
+      <c r="C43" s="3">
+        <v>52.075899999999997</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.744031</v>
+      </c>
+      <c r="E43" s="3">
+        <v>53.170400000000001</v>
+      </c>
+      <c r="F43" s="3">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="G43" s="3">
+        <v>9.3625000000000007</v>
+      </c>
+      <c r="H43" s="3">
+        <v>49.956000000000003</v>
+      </c>
+      <c r="I43" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="J43" s="3">
+        <v>14.75</v>
+      </c>
+      <c r="K43" s="3">
+        <v>34.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3">
+        <v>-3.6941600000000001</v>
+      </c>
+      <c r="C44" s="3">
+        <v>65.611099999999993</v>
+      </c>
+      <c r="D44" s="3">
+        <v>-1.4380900000000001</v>
+      </c>
+      <c r="E44" s="3">
+        <v>36.886400000000002</v>
+      </c>
+      <c r="F44" s="3">
+        <v>-3.7749999999999999</v>
+      </c>
+      <c r="G44" s="3">
+        <v>2.7124999999999999</v>
+      </c>
+      <c r="H44" s="3">
+        <v>74.963999999999999</v>
+      </c>
+      <c r="I44" s="3">
+        <v>27.65</v>
+      </c>
+      <c r="J44" s="3">
+        <v>19.75</v>
+      </c>
+      <c r="K44" s="3">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3">
+        <v>-7.3853799999999996</v>
+      </c>
+      <c r="C45" s="3">
+        <v>43.7941</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.68827899999999997</v>
+      </c>
+      <c r="E45" s="3">
+        <v>36.476700000000001</v>
+      </c>
+      <c r="F45" s="3">
+        <v>-0.58750000000000002</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1.0625</v>
+      </c>
+      <c r="H45" s="3">
+        <v>75.866799999999998</v>
+      </c>
+      <c r="I45" s="3">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="J45" s="3">
+        <v>20.25</v>
+      </c>
+      <c r="K45" s="3">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3">
+        <v>-13.4565</v>
+      </c>
+      <c r="C46" s="3">
+        <v>48.8461</v>
+      </c>
+      <c r="D46" s="3">
+        <v>-0.37657600000000002</v>
+      </c>
+      <c r="E46" s="3">
+        <v>58.341200000000001</v>
+      </c>
+      <c r="F46" s="3">
+        <v>-3.7625000000000002</v>
+      </c>
+      <c r="G46" s="3">
+        <v>6.5625</v>
+      </c>
+      <c r="H46" s="3">
+        <v>44.786200000000001</v>
+      </c>
+      <c r="I46" s="3">
+        <v>24.75</v>
+      </c>
+      <c r="J46" s="3">
         <v>12</v>
       </c>
-      <c r="B39" s="4">
+      <c r="K46" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3">
+        <v>-24.1509</v>
+      </c>
+      <c r="C47" s="3">
+        <v>41.458500000000001</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.1940299999999999</v>
+      </c>
+      <c r="E47" s="3">
+        <v>63.174599999999998</v>
+      </c>
+      <c r="F47" s="3">
+        <v>2.6749999999999998</v>
+      </c>
+      <c r="G47" s="3">
+        <v>1.3125</v>
+      </c>
+      <c r="H47" s="3">
+        <v>40.6571</v>
+      </c>
+      <c r="I47" s="3">
+        <v>22</v>
+      </c>
+      <c r="J47" s="3">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="K47" s="3">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3">
+        <v>-2.8466</v>
+      </c>
+      <c r="C48" s="3">
+        <v>52.880800000000001</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1.1017999999999999</v>
+      </c>
+      <c r="E48" s="3">
+        <v>53.339500000000001</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1.0874999999999999</v>
+      </c>
+      <c r="G48" s="3">
+        <v>2.1124999999999998</v>
+      </c>
+      <c r="H48" s="3">
+        <v>49.772399999999998</v>
+      </c>
+      <c r="I48" s="3">
+        <v>38</v>
+      </c>
+      <c r="J48" s="3">
+        <v>14.35</v>
+      </c>
+      <c r="K48" s="3">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3">
+        <v>-17.808199999999999</v>
+      </c>
+      <c r="C49" s="3">
+        <v>31.711300000000001</v>
+      </c>
+      <c r="D49" s="3">
+        <v>2.96618</v>
+      </c>
+      <c r="E49" s="3">
+        <v>55.168700000000001</v>
+      </c>
+      <c r="F49" s="3">
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="G49" s="3">
+        <v>4.2625000000000002</v>
+      </c>
+      <c r="H49" s="3">
+        <v>47.852400000000003</v>
+      </c>
+      <c r="I49" s="3">
+        <v>15.15</v>
+      </c>
+      <c r="J49" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="K49" s="3">
+        <v>32.950000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3">
+        <v>-4.8871599999999997</v>
+      </c>
+      <c r="C50" s="3">
+        <v>63.703600000000002</v>
+      </c>
+      <c r="D50" s="3">
+        <v>-0.63002199999999997</v>
+      </c>
+      <c r="E50" s="3">
+        <v>58.093400000000003</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1.075</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.65000100000000005</v>
+      </c>
+      <c r="H50" s="3">
+        <v>45.014699999999998</v>
+      </c>
+      <c r="I50" s="3">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J50" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="K50" s="3">
+        <v>13.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3">
+        <v>-15.104900000000001</v>
+      </c>
+      <c r="C51" s="3">
+        <v>49.213799999999999</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.66833799999999999</v>
+      </c>
+      <c r="E51" s="3">
+        <v>60.225999999999999</v>
+      </c>
+      <c r="F51" s="3">
+        <v>-5.4749999999999996</v>
+      </c>
+      <c r="G51" s="3">
+        <v>3.0249999999999999</v>
+      </c>
+      <c r="H51" s="3">
+        <v>43.104700000000001</v>
+      </c>
+      <c r="I51" s="3">
+        <v>13.55</v>
+      </c>
+      <c r="J51" s="3">
+        <v>18.75</v>
+      </c>
+      <c r="K51" s="3">
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
         <f>MIN(B2:B36)</f>
         <v>-35.741399999999999</v>
       </c>
-      <c r="C39" s="4">
-        <f t="shared" ref="C39:K39" si="1">MIN(C2:C36)</f>
+      <c r="C53" s="4">
+        <f t="shared" ref="C53:K53" si="0">MIN(C2:C36)</f>
         <v>22.553699999999999</v>
       </c>
-      <c r="D39" s="4">
-        <f t="shared" si="1"/>
+      <c r="D53" s="4">
+        <f t="shared" si="0"/>
         <v>-4.0158399999999999</v>
       </c>
-      <c r="E39" s="4">
-        <f t="shared" si="1"/>
+      <c r="E53" s="4">
+        <f t="shared" si="0"/>
         <v>20.684999999999999</v>
       </c>
-      <c r="F39" s="4">
-        <f t="shared" si="1"/>
+      <c r="F53" s="4">
+        <f t="shared" si="0"/>
         <v>-7.7</v>
       </c>
-      <c r="G39" s="4">
-        <f t="shared" si="1"/>
-        <v>-7.5374999999999996</v>
-      </c>
-      <c r="H39" s="4">
-        <f t="shared" si="1"/>
+      <c r="G53" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.4625000000000004</v>
+      </c>
+      <c r="H53" s="4">
+        <f t="shared" si="0"/>
         <v>26.136900000000001</v>
       </c>
-      <c r="I39" s="4">
-        <f t="shared" si="1"/>
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="J39" s="4">
-        <f t="shared" si="1"/>
+      <c r="I53" s="4">
+        <f t="shared" si="0"/>
+        <v>8.25</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
-      <c r="K39" s="4">
-        <f t="shared" si="1"/>
+      <c r="K53" s="4">
+        <f t="shared" si="0"/>
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="4">
+        <f>MAX(B4:B38)</f>
+        <v>38.5</v>
+      </c>
+      <c r="C54" s="4">
+        <f>MAX(C4:C38)</f>
+        <v>74.290199999999999</v>
+      </c>
+      <c r="D54" s="4">
+        <f>MAX(D4:D38)</f>
+        <v>13.81</v>
+      </c>
+      <c r="E54" s="4">
+        <f>MAX(E4:E38)</f>
+        <v>87.4529</v>
+      </c>
+      <c r="F54" s="4">
+        <f>MAX(F4:F38)</f>
+        <v>12.137499999999999</v>
+      </c>
+      <c r="G54" s="4">
+        <f>MAX(G4:G38)</f>
+        <v>13.824999999999999</v>
+      </c>
+      <c r="H54" s="4">
+        <f>MAX(H4:H38)</f>
+        <v>136.988</v>
+      </c>
+      <c r="I54" s="4">
+        <f>MAX(I4:I38)</f>
+        <v>48.6</v>
+      </c>
+      <c r="J54" s="4">
+        <f>MAX(J4:J38)</f>
+        <v>44.05</v>
+      </c>
+      <c r="K54" s="4">
+        <f>MAX(K4:K38)</f>
+        <v>45.65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>20</v>
+      </c>
+      <c r="D56">
+        <v>-10</v>
+      </c>
+      <c r="E56">
+        <v>20</v>
+      </c>
+      <c r="F56">
+        <v>-15</v>
+      </c>
+      <c r="G56">
+        <v>-15</v>
+      </c>
+      <c r="I56">
+        <v>4</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>-40</v>
+      </c>
+      <c r="C57">
+        <v>70</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
+      <c r="E57">
+        <v>90</v>
+      </c>
+      <c r="F57">
+        <v>15</v>
+      </c>
+      <c r="G57">
+        <v>15</v>
+      </c>
+      <c r="I57">
+        <v>50</v>
+      </c>
+      <c r="J57">
+        <v>50</v>
+      </c>
+      <c r="K57">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="83" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add ShiftImage and VanishigPointPM
</commit_message>
<xml_diff>
--- a/parameter_estimation.xlsx
+++ b/parameter_estimation.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Original photos" sheetId="1" r:id="rId1"/>
     <sheet name="Small photos" sheetId="2" r:id="rId2"/>
+    <sheet name="Centered photos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
   <si>
     <t>No.</t>
   </si>
@@ -145,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -156,7 +157,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,11 +464,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,48 +628,48 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>-24.174700000000001</v>
+        <v>-24.6008</v>
       </c>
       <c r="C4" s="3">
-        <v>-39.938299999999998</v>
+        <v>-39.967300000000002</v>
       </c>
       <c r="D4" s="3">
-        <v>1.54512</v>
+        <v>1.5579499999999999</v>
       </c>
       <c r="E4" s="3">
-        <v>65.630499999999998</v>
+        <v>64.941400000000002</v>
       </c>
       <c r="F4" s="3">
-        <v>-1.8823700000000001</v>
+        <v>-1.9431799999999999</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>-4.8552606803766864E-2</v>
+        <v>-4.9461774400875617E-2</v>
       </c>
       <c r="H4" s="3">
-        <v>-0.17466300000000001</v>
+        <v>0.53104899999999999</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="1"/>
-        <v>-4.5051419020523762E-3</v>
+        <v>1.3517340562279665E-2</v>
       </c>
       <c r="J4" s="3">
-        <v>38.7697</v>
+        <v>39.286499999999997</v>
       </c>
       <c r="K4" s="3">
-        <v>3.12051E-2</v>
+        <v>2.72728E-2</v>
       </c>
       <c r="L4" s="3">
-        <v>-1.6986500000000002E-2</v>
+        <v>-7.58028E-4</v>
       </c>
       <c r="M4" s="3">
         <v>20.75</v>
       </c>
       <c r="N4" s="3">
-        <v>35.65</v>
+        <v>36.65</v>
       </c>
       <c r="O4" s="3">
-        <v>12.4</v>
+        <v>12.55</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>25.05</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1309,56 +1309,56 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>-6.8361999999999998</v>
+        <v>-5.5978500000000002</v>
       </c>
       <c r="C18" s="3">
-        <v>-34.031700000000001</v>
+        <v>-32.650399999999998</v>
       </c>
       <c r="D18" s="3">
-        <v>-1.0037</v>
+        <v>-0.92155799999999999</v>
       </c>
       <c r="E18" s="3">
-        <v>40.767699999999998</v>
+        <v>41.821199999999997</v>
       </c>
       <c r="F18" s="3">
-        <v>-10.7629</v>
+        <v>-7.9486999999999997</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="0"/>
-        <v>-0.15996961990698697</v>
+        <v>-0.12147994412536947</v>
       </c>
       <c r="H18" s="3">
-        <v>3.6650999999999998</v>
+        <v>2.1839400000000002</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="1"/>
-        <v>5.447459828866736E-2</v>
+        <v>3.3377144586304607E-2</v>
       </c>
       <c r="J18" s="3">
-        <v>67.280900000000003</v>
+        <v>65.432199999999995</v>
       </c>
       <c r="K18" s="3">
-        <v>-0.64301399999999997</v>
+        <v>-0.53044800000000003</v>
       </c>
       <c r="L18" s="3">
-        <v>8.7604000000000001E-2</v>
+        <v>2.9857499999999999E-2</v>
       </c>
       <c r="M18" s="3">
-        <v>17</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="N18" s="3">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="O18" s="3">
-        <v>24.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>25.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>18.149999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>18.649999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1554,56 +1554,56 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>-8.8099299999999996</v>
+        <v>-7.7675400000000003</v>
       </c>
       <c r="C23" s="3">
-        <v>-44.231400000000001</v>
+        <v>-45.964300000000001</v>
       </c>
       <c r="D23" s="3">
-        <v>-1.5536300000000001</v>
+        <v>-1.6054299999999999</v>
       </c>
       <c r="E23" s="3">
-        <v>34.930599999999998</v>
+        <v>34.867600000000003</v>
       </c>
       <c r="F23" s="3">
-        <v>0.55301699999999998</v>
+        <v>-4.4307600000000003</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="0"/>
-        <v>6.9599006262459472E-3</v>
+        <v>-5.5655402672508437E-2</v>
       </c>
       <c r="H23" s="3">
-        <v>1.8175300000000001</v>
+        <v>0.399586</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="1"/>
-        <v>2.2874212158434184E-2</v>
+        <v>5.0192562296980546E-3</v>
       </c>
       <c r="J23" s="3">
-        <v>79.457599999999999</v>
+        <v>79.610600000000005</v>
       </c>
       <c r="K23" s="3">
-        <v>-3.6379300000000003E-2</v>
+        <v>-0.22922999999999999</v>
       </c>
       <c r="L23" s="3">
-        <v>6.2701099999999996E-2</v>
+        <v>4.4834599999999999E-3</v>
       </c>
       <c r="M23" s="3">
-        <v>24.35</v>
+        <v>25.55</v>
       </c>
       <c r="N23" s="3">
-        <v>17.45</v>
+        <v>17.350000000000001</v>
       </c>
       <c r="O23" s="3">
-        <v>32.700000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>31.35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>29.85</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1801,9 +1801,8 @@
       <c r="P27" t="s">
         <v>14</v>
       </c>
-      <c r="R27" s="8"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1852,7 +1851,7 @@
         <v>46.55</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>28.05</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1999,56 +1998,56 @@
         <v>22.35</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>-3.6654800000000001</v>
+        <v>-1.65489</v>
       </c>
       <c r="C32" s="3">
-        <v>-39.168100000000003</v>
+        <v>-35.976700000000001</v>
       </c>
       <c r="D32" s="3">
-        <v>0.88592800000000005</v>
+        <v>0.85610699999999995</v>
       </c>
       <c r="E32" s="3">
-        <v>44.593699999999998</v>
+        <v>45.545200000000001</v>
       </c>
       <c r="F32" s="3">
-        <v>0.42738999999999999</v>
+        <v>6.6778399999999998</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
-        <v>7.0103238208963055E-3</v>
+        <v>0.11213404016301637</v>
       </c>
       <c r="H32" s="3">
-        <v>1.5341400000000001</v>
+        <v>-1.0236400000000001</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="1"/>
-        <v>2.516394437537111E-2</v>
+        <v>-1.7188924693084903E-2</v>
       </c>
       <c r="J32" s="3">
-        <v>60.965800000000002</v>
+        <v>59.552300000000002</v>
       </c>
       <c r="K32" s="3">
-        <v>0.107096</v>
+        <v>0.369114</v>
       </c>
       <c r="L32" s="3">
-        <v>8.6365800000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="M32" s="3">
-        <v>38.1</v>
+        <v>35.85</v>
       </c>
       <c r="N32" s="3">
-        <v>10.85</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="O32" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2099,9 +2098,8 @@
       <c r="P33" t="s">
         <v>14</v>
       </c>
-      <c r="R33" s="8"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2150,7 +2148,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2199,7 +2197,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2248,7 +2246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2300,7 +2298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2401,7 +2399,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2453,7 +2451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2502,7 +2500,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2551,7 +2549,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2600,7 +2598,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2649,7 +2647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2698,7 +2696,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2747,7 +2745,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2796,53 +2794,53 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="3">
-        <v>-0.119203</v>
+        <v>-2.2913199999999998</v>
       </c>
       <c r="C48" s="3">
-        <v>-10.529</v>
+        <v>-32.545999999999999</v>
       </c>
       <c r="D48" s="3">
-        <v>0.67666199999999999</v>
+        <v>0.74732200000000004</v>
       </c>
       <c r="E48" s="3">
-        <v>106.717</v>
+        <v>56.158700000000003</v>
       </c>
       <c r="F48" s="3">
-        <v>35.276600000000002</v>
+        <v>8.7867200000000008</v>
       </c>
       <c r="G48" s="3">
         <f t="shared" si="0"/>
-        <v>1.8971115736035151</v>
+        <v>0.18750402782668077</v>
       </c>
       <c r="H48" s="3">
-        <v>0.51583400000000001</v>
+        <v>2.18933</v>
       </c>
       <c r="I48" s="3">
         <f t="shared" si="1"/>
-        <v>2.7740617050911812E-2</v>
+        <v>4.6719161785260824E-2</v>
       </c>
       <c r="J48" s="3">
-        <v>18.594899999999999</v>
+        <v>46.861499999999999</v>
       </c>
       <c r="K48" s="3">
-        <v>1.36856</v>
+        <v>0.30846899999999999</v>
       </c>
       <c r="L48" s="3">
-        <v>-4.9366699999999999E-2</v>
+        <v>2.1573200000000001E-2</v>
       </c>
       <c r="M48" s="3">
-        <v>3.3</v>
+        <v>9.6</v>
       </c>
       <c r="N48" s="3">
-        <v>13.45</v>
+        <v>13.4</v>
       </c>
       <c r="O48" s="3">
-        <v>46.65</v>
+        <v>40.15</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3047,7 +3045,7 @@
       </c>
       <c r="J53" s="4">
         <f t="shared" si="2"/>
-        <v>18.594899999999999</v>
+        <v>28.910299999999999</v>
       </c>
       <c r="K53" s="4">
         <f t="shared" si="2"/>
@@ -3059,7 +3057,7 @@
       </c>
       <c r="M53" s="4">
         <f t="shared" si="2"/>
-        <v>3.3</v>
+        <v>6.25</v>
       </c>
       <c r="N53" s="4">
         <f t="shared" si="2"/>
@@ -3080,7 +3078,7 @@
       </c>
       <c r="C54" s="4">
         <f t="shared" ref="C54:O54" si="4">MAX(C2:C51)</f>
-        <v>-10.529</v>
+        <v>-16.785499999999999</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="4"/>
@@ -3088,15 +3086,15 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="4"/>
-        <v>106.717</v>
+        <v>81.7029</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="4"/>
-        <v>35.276600000000002</v>
+        <v>8.7867200000000008</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" ref="G54:I54" si="5">MAX(G2:G51)</f>
-        <v>1.8971115736035151</v>
+        <v>0.20252981210558732</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="5"/>
@@ -3112,7 +3110,7 @@
       </c>
       <c r="K54" s="4">
         <f t="shared" si="4"/>
-        <v>1.36856</v>
+        <v>0.40425499999999998</v>
       </c>
       <c r="L54" s="4">
         <f t="shared" si="4"/>
@@ -3128,7 +3126,7 @@
       </c>
       <c r="O54" s="4">
         <f t="shared" si="4"/>
-        <v>46.65</v>
+        <v>46.55</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3220,7 +3218,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="83" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="60" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4203,4 +4201,1850 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.5850900000000001</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-25.5595</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.98457099999999997</v>
+      </c>
+      <c r="E2" s="3">
+        <v>85.751999999999995</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5.45261</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-5.9581799999999996</v>
+      </c>
+      <c r="H2" s="3">
+        <v>26.925799999999999</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.8699999999999999E-4</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-8.2700000000000004E-4</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L2" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="M2" s="3">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-10.0106</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-35.862200000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-2.9799699999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <v>76.456999999999994</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-3.4883600000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.21085699999999999</v>
+      </c>
+      <c r="H3" s="3">
+        <v>31.736799999999999</v>
+      </c>
+      <c r="I3" s="3">
+        <v>9.1799999999999998E-4</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-1.2359999999999999E-3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>14.25</v>
+      </c>
+      <c r="L3" s="3">
+        <v>10.95</v>
+      </c>
+      <c r="M3" s="3">
+        <v>22.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-24.174800000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-39.938699999999997</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.54497</v>
+      </c>
+      <c r="E4" s="3">
+        <v>66.461799999999997</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-1.71607</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.12803300000000001</v>
+      </c>
+      <c r="H4" s="3">
+        <v>38.159100000000002</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.1770000000000001E-3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>-9.7400000000000004E-4</v>
+      </c>
+      <c r="K4" s="3">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="M4" s="3">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-12.823499999999999</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-18.628</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.75779</v>
+      </c>
+      <c r="E5" s="3">
+        <v>52.271099999999997</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.34873</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.2813000000000001</v>
+      </c>
+      <c r="H5" s="3">
+        <v>50.951300000000003</v>
+      </c>
+      <c r="I5" s="3">
+        <v>9.1933499999999997E-4</v>
+      </c>
+      <c r="J5" s="3">
+        <v>-4.40612E-4</v>
+      </c>
+      <c r="K5" s="3">
+        <v>14.85</v>
+      </c>
+      <c r="L5" s="3">
+        <v>22.25</v>
+      </c>
+      <c r="M5" s="3">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-15.5085</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-34.307000000000002</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0063900000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>46.6267</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-0.55500300000000002</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-0.93716999999999995</v>
+      </c>
+      <c r="H6" s="3">
+        <v>58.012099999999997</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.1774000000000001E-3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-9.4427300000000003E-4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="M6" s="3">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-22.828499999999998</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-44.211500000000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.1694200000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>52.517299999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5.4611799999999997</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.2174700000000001</v>
+      </c>
+      <c r="H7" s="3">
+        <v>50.675699999999999</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.0874000000000001E-3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>-4.51216E-4</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3.55</v>
+      </c>
+      <c r="L7" s="3">
+        <v>35.5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>-5.4821799999999996</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-68.405299999999997</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-0.650362</v>
+      </c>
+      <c r="E8" s="3">
+        <v>54.357100000000003</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4.8399400000000004</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1.9019999999999999</v>
+      </c>
+      <c r="H8" s="3">
+        <v>48.689599999999999</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.35757E-3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>-1.2848200000000001E-3</v>
+      </c>
+      <c r="K8" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="L8" s="3">
+        <v>8.35</v>
+      </c>
+      <c r="M8" s="3">
+        <v>43.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>-15.3634</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-49.007899999999999</v>
+      </c>
+      <c r="D9" s="3">
+        <v>-0.28124500000000002</v>
+      </c>
+      <c r="E9" s="3">
+        <v>54.301400000000001</v>
+      </c>
+      <c r="F9" s="3">
+        <v>-2.1589399999999999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1.3823700000000001</v>
+      </c>
+      <c r="H9" s="3">
+        <v>48.747799999999998</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.2597400000000001E-3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>-9.6760599999999998E-4</v>
+      </c>
+      <c r="K9" s="3">
+        <v>16.75</v>
+      </c>
+      <c r="L9" s="3">
+        <v>25</v>
+      </c>
+      <c r="M9" s="3">
+        <v>14.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>-12.2773</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-28.586300000000001</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.64634899999999995</v>
+      </c>
+      <c r="E10" s="3">
+        <v>61.648699999999998</v>
+      </c>
+      <c r="F10" s="3">
+        <v>-4.5033700000000003</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5.1962799999999998</v>
+      </c>
+      <c r="H10" s="3">
+        <v>41.897399999999998</v>
+      </c>
+      <c r="I10" s="3">
+        <v>8.05327E-4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>-1.6339099999999999E-3</v>
+      </c>
+      <c r="K10" s="3">
+        <v>22.4</v>
+      </c>
+      <c r="L10" s="3">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="M10" s="3">
+        <v>12.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>-11.444599999999999</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-55.256</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-3.2433100000000001</v>
+      </c>
+      <c r="E11" s="3">
+        <v>22.186</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.617313</v>
+      </c>
+      <c r="G11" s="3">
+        <v>13.545999999999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>127.508</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.71002E-3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>-3.4708600000000001E-3</v>
+      </c>
+      <c r="K11" s="3">
+        <v>11.45</v>
+      </c>
+      <c r="L11" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="M11" s="3">
+        <v>11.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>-11.703900000000001</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-44.5261</v>
+      </c>
+      <c r="D12" s="3">
+        <v>-1.69292</v>
+      </c>
+      <c r="E12" s="3">
+        <v>85.028499999999994</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4.3195199999999998</v>
+      </c>
+      <c r="G12" s="3">
+        <v>-1.1526799999999999</v>
+      </c>
+      <c r="H12" s="3">
+        <v>27.269100000000002</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.8341100000000001E-4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>-1.0496100000000001E-3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>14.3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="M12" s="3">
+        <v>34.049999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-6.4803100000000002</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-34.8872</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.37063499999999999</v>
+      </c>
+      <c r="E13" s="3">
+        <v>53.489800000000002</v>
+      </c>
+      <c r="F13" s="3">
+        <v>5.4268799999999997</v>
+      </c>
+      <c r="G13" s="3">
+        <v>-1.11158</v>
+      </c>
+      <c r="H13" s="3">
+        <v>49.61</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.8503E-3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>-6.7303899999999995E-4</v>
+      </c>
+      <c r="K13" s="3">
+        <v>15.6</v>
+      </c>
+      <c r="L13" s="3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="M13" s="3">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>-7.3946699999999996</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-56.5261</v>
+      </c>
+      <c r="D14" s="3">
+        <v>-1.80402</v>
+      </c>
+      <c r="E14" s="3">
+        <v>72.698099999999997</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1.3741000000000001</v>
+      </c>
+      <c r="G14" s="3">
+        <v>-0.14761199999999999</v>
+      </c>
+      <c r="H14" s="3">
+        <v>33.9724</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3.4660300000000002E-4</v>
+      </c>
+      <c r="J14" s="3">
+        <v>-9.2949000000000005E-4</v>
+      </c>
+      <c r="K14" s="3">
+        <v>19.5</v>
+      </c>
+      <c r="L14" s="3">
+        <v>9.15</v>
+      </c>
+      <c r="M14" s="3">
+        <v>32.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>-20.349299999999999</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-35.937899999999999</v>
+      </c>
+      <c r="D15" s="3">
+        <v>-5.9359000000000002E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>56.676200000000001</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3.5611700000000002</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.77144599999999997</v>
+      </c>
+      <c r="H15" s="3">
+        <v>46.356200000000001</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.67453E-3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>-1.83468E-3</v>
+      </c>
+      <c r="K15" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="L15" s="3">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="M15" s="3">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>-11.853400000000001</v>
+      </c>
+      <c r="C16" s="3">
+        <v>-54.779899999999998</v>
+      </c>
+      <c r="D16" s="3">
+        <v>-2.0862799999999999</v>
+      </c>
+      <c r="E16" s="3">
+        <v>46.990900000000003</v>
+      </c>
+      <c r="F16" s="3">
+        <v>-0.58065500000000003</v>
+      </c>
+      <c r="G16" s="3">
+        <v>4.0510200000000003</v>
+      </c>
+      <c r="H16" s="3">
+        <v>57.508600000000001</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1.4887800000000001E-3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>-1.30422E-3</v>
+      </c>
+      <c r="K16" s="3">
+        <v>18.5</v>
+      </c>
+      <c r="L16" s="3">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="M16" s="3">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>-4.3539199999999996</v>
+      </c>
+      <c r="C17" s="3">
+        <v>-46.119599999999998</v>
+      </c>
+      <c r="D17" s="3">
+        <v>-3.0783499999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>71.393299999999996</v>
+      </c>
+      <c r="F17" s="3">
+        <v>-4.6290199999999997</v>
+      </c>
+      <c r="G17" s="3">
+        <v>-4.3065100000000003</v>
+      </c>
+      <c r="H17" s="3">
+        <v>34.795499999999997</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1.8184900000000001E-4</v>
+      </c>
+      <c r="J17" s="3">
+        <v>-2.6309499999999997E-4</v>
+      </c>
+      <c r="K17" s="3">
+        <v>10.15</v>
+      </c>
+      <c r="L17" s="3">
+        <v>14.75</v>
+      </c>
+      <c r="M17" s="3">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>-5.5989100000000001</v>
+      </c>
+      <c r="C18" s="3">
+        <v>-32.650300000000001</v>
+      </c>
+      <c r="D18" s="3">
+        <v>-0.92176800000000003</v>
+      </c>
+      <c r="E18" s="3">
+        <v>60.622799999999998</v>
+      </c>
+      <c r="F18" s="3">
+        <v>-5.3935399999999998</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="H18" s="3">
+        <v>42.762799999999999</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3.6098800000000002E-4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>-1.1899600000000001E-3</v>
+      </c>
+      <c r="K18" s="3">
+        <v>12</v>
+      </c>
+      <c r="L18" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="M18" s="3">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-1.89645</v>
+      </c>
+      <c r="C19" s="3">
+        <v>-34.1828</v>
+      </c>
+      <c r="D19" s="3">
+        <v>-1.77752</v>
+      </c>
+      <c r="E19" s="3">
+        <v>33.865699999999997</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.91844999999999999</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-3.7922899999999999</v>
+      </c>
+      <c r="H19" s="3">
+        <v>82.115399999999994</v>
+      </c>
+      <c r="I19" s="3">
+        <v>-3.59472E-4</v>
+      </c>
+      <c r="J19" s="3">
+        <v>-9.18972E-4</v>
+      </c>
+      <c r="K19" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="L19" s="3">
+        <v>13.15</v>
+      </c>
+      <c r="M19" s="3">
+        <v>12.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>-14.326700000000001</v>
+      </c>
+      <c r="C20" s="3">
+        <v>-42.782600000000002</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.58684899999999995</v>
+      </c>
+      <c r="E20" s="3">
+        <v>76.810500000000005</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-1.3372999999999999</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.45202999999999999</v>
+      </c>
+      <c r="H20" s="3">
+        <v>31.536200000000001</v>
+      </c>
+      <c r="I20" s="3">
+        <v>6.1549700000000001E-4</v>
+      </c>
+      <c r="J20" s="3">
+        <v>-8.7632499999999996E-4</v>
+      </c>
+      <c r="K20" s="3">
+        <v>23.55</v>
+      </c>
+      <c r="L20" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>-14.006600000000001</v>
+      </c>
+      <c r="C21" s="3">
+        <v>-38.9191</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.4511000000000001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>54.340600000000002</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.59348999999999996</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2.3921399999999999</v>
+      </c>
+      <c r="H21" s="3">
+        <v>48.706800000000001</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1.7121E-3</v>
+      </c>
+      <c r="J21" s="3">
+        <v>-6.2209799999999997E-4</v>
+      </c>
+      <c r="K21" s="3">
+        <v>30.7</v>
+      </c>
+      <c r="L21" s="3">
+        <v>23.1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>-9.66798</v>
+      </c>
+      <c r="C22" s="3">
+        <v>-23.092400000000001</v>
+      </c>
+      <c r="D22" s="3">
+        <v>5.1007199999999999</v>
+      </c>
+      <c r="E22" s="3">
+        <v>68.058899999999994</v>
+      </c>
+      <c r="F22" s="3">
+        <v>3.2394799999999999</v>
+      </c>
+      <c r="G22" s="3">
+        <v>-2.4668399999999999</v>
+      </c>
+      <c r="H22" s="3">
+        <v>37.023000000000003</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>-8.0371700000000002E-4</v>
+      </c>
+      <c r="K22" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="L22" s="3">
+        <v>22.6</v>
+      </c>
+      <c r="M22" s="3">
+        <v>10.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>-7.7674399999999997</v>
+      </c>
+      <c r="C23" s="3">
+        <v>-45.963799999999999</v>
+      </c>
+      <c r="D23" s="3">
+        <v>-1.6052999999999999</v>
+      </c>
+      <c r="E23" s="3">
+        <v>42.176099999999998</v>
+      </c>
+      <c r="F23" s="3">
+        <v>-3.4973399999999999</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.29487999999999998</v>
+      </c>
+      <c r="H23" s="3">
+        <v>64.829300000000003</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1.0264E-3</v>
+      </c>
+      <c r="J23" s="3">
+        <v>-3.92307E-4</v>
+      </c>
+      <c r="K23" s="3">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="L23" s="3">
+        <v>14.05</v>
+      </c>
+      <c r="M23" s="3">
+        <v>25.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3">
+        <v>-31.913699999999999</v>
+      </c>
+      <c r="C24" s="3">
+        <v>-49.090699999999998</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.99974799999999997</v>
+      </c>
+      <c r="E24" s="3">
+        <v>81.159199999999998</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.249113</v>
+      </c>
+      <c r="G24" s="3">
+        <v>11.86</v>
+      </c>
+      <c r="H24" s="3">
+        <v>29.189</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1.0345300000000001E-3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>-1.48485E-3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>19.95</v>
+      </c>
+      <c r="L24" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="M24" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>-10.021100000000001</v>
+      </c>
+      <c r="C25" s="3">
+        <v>-47.657499999999999</v>
+      </c>
+      <c r="D25" s="3">
+        <v>-0.35420699999999999</v>
+      </c>
+      <c r="E25" s="3">
+        <v>54.495800000000003</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2.7272799999999999</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1.34213</v>
+      </c>
+      <c r="H25" s="3">
+        <v>48.544800000000002</v>
+      </c>
+      <c r="I25" s="3">
+        <v>9.0384199999999997E-4</v>
+      </c>
+      <c r="J25" s="3">
+        <v>-8.9471699999999995E-4</v>
+      </c>
+      <c r="K25" s="3">
+        <v>27.55</v>
+      </c>
+      <c r="L25" s="3">
+        <v>15.95</v>
+      </c>
+      <c r="M25" s="3">
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3">
+        <v>-7.4583000000000004</v>
+      </c>
+      <c r="C26" s="3">
+        <v>-42.438299999999998</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.205513</v>
+      </c>
+      <c r="E26" s="3">
+        <v>56.669899999999998</v>
+      </c>
+      <c r="F26" s="3">
+        <v>-1.0325899999999999</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.22012100000000001</v>
+      </c>
+      <c r="H26" s="3">
+        <v>46.362299999999998</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.20897E-3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>-6.8269100000000003E-4</v>
+      </c>
+      <c r="K26" s="3">
+        <v>28.15</v>
+      </c>
+      <c r="L26" s="3">
+        <v>13.45</v>
+      </c>
+      <c r="M26" s="3">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3">
+        <v>-8.5511300000000006</v>
+      </c>
+      <c r="C28" s="3">
+        <v>-39.551200000000001</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.48707099999999998</v>
+      </c>
+      <c r="E28" s="3">
+        <v>57.546599999999998</v>
+      </c>
+      <c r="F28" s="3">
+        <v>6.4812500000000002</v>
+      </c>
+      <c r="G28" s="3">
+        <v>4.0910399999999996</v>
+      </c>
+      <c r="H28" s="3">
+        <v>45.525100000000002</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1.0273299999999999E-3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>-8.7343299999999996E-4</v>
+      </c>
+      <c r="K28" s="3">
+        <v>13.75</v>
+      </c>
+      <c r="L28" s="3">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="M28" s="3">
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
+        <v>-4.1684700000000001</v>
+      </c>
+      <c r="C29" s="3">
+        <v>-51.854300000000002</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3.6112299999999999</v>
+      </c>
+      <c r="E29" s="3">
+        <v>53.5625</v>
+      </c>
+      <c r="F29" s="3">
+        <v>-0.209896</v>
+      </c>
+      <c r="G29" s="3">
+        <v>-1.31962</v>
+      </c>
+      <c r="H29" s="3">
+        <v>49.5319</v>
+      </c>
+      <c r="I29" s="3">
+        <v>3.54149E-4</v>
+      </c>
+      <c r="J29" s="3">
+        <v>-1.61713E-3</v>
+      </c>
+      <c r="K29" s="3">
+        <v>28.9</v>
+      </c>
+      <c r="L29" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="M29" s="3">
+        <v>22.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>-6.7791899999999998</v>
+      </c>
+      <c r="C30" s="3">
+        <v>-51.179600000000001</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-2.01024</v>
+      </c>
+      <c r="E30" s="3">
+        <v>55.123899999999999</v>
+      </c>
+      <c r="F30" s="3">
+        <v>-4.8654900000000003</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.17063200000000001</v>
+      </c>
+      <c r="H30" s="3">
+        <v>47.898000000000003</v>
+      </c>
+      <c r="I30" s="3">
+        <v>4.3551199999999999E-4</v>
+      </c>
+      <c r="J30" s="3">
+        <v>-6.2222700000000004E-4</v>
+      </c>
+      <c r="K30" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="L30" s="3">
+        <v>7.85</v>
+      </c>
+      <c r="M30" s="3">
+        <v>25.65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>-16.298300000000001</v>
+      </c>
+      <c r="C31" s="3">
+        <v>-57.362000000000002</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.334262</v>
+      </c>
+      <c r="E31" s="3">
+        <v>51.137300000000003</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1.59348</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.55721200000000004</v>
+      </c>
+      <c r="H31" s="3">
+        <v>52.252299999999998</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1.8442199999999999E-3</v>
+      </c>
+      <c r="J31" s="3">
+        <v>-1.8890000000000001E-3</v>
+      </c>
+      <c r="K31" s="3">
+        <v>21.649899999999999</v>
+      </c>
+      <c r="L31" s="3">
+        <v>29.5</v>
+      </c>
+      <c r="M31" s="3">
+        <v>21.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>-1.65526</v>
+      </c>
+      <c r="C32" s="3">
+        <v>-35.979199999999999</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.85602599999999995</v>
+      </c>
+      <c r="E32" s="3">
+        <v>59.734099999999998</v>
+      </c>
+      <c r="F32" s="3">
+        <v>5.0146199999999999</v>
+      </c>
+      <c r="G32" s="3">
+        <v>-0.77546700000000002</v>
+      </c>
+      <c r="H32" s="3">
+        <v>43.534300000000002</v>
+      </c>
+      <c r="I32" s="3">
+        <v>6.77401E-4</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>25.85</v>
+      </c>
+      <c r="L32" s="3">
+        <v>7.35</v>
+      </c>
+      <c r="M32" s="3">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>-0.94887299999999997</v>
+      </c>
+      <c r="C34" s="3">
+        <v>-44.548299999999998</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.8497399999999999</v>
+      </c>
+      <c r="E34" s="3">
+        <v>55.238799999999998</v>
+      </c>
+      <c r="F34" s="3">
+        <v>4.64133</v>
+      </c>
+      <c r="G34" s="3">
+        <v>-1.76224</v>
+      </c>
+      <c r="H34" s="3">
+        <v>47.781199999999998</v>
+      </c>
+      <c r="I34" s="3">
+        <v>7.9066E-4</v>
+      </c>
+      <c r="J34" s="3">
+        <v>-6.1946699999999996E-4</v>
+      </c>
+      <c r="K34" s="3">
+        <v>31.05</v>
+      </c>
+      <c r="L34" s="3">
+        <v>9.15</v>
+      </c>
+      <c r="M34" s="3">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3">
+        <v>-11.602399999999999</v>
+      </c>
+      <c r="C36" s="3">
+        <v>-39.762300000000003</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.8700699999999999</v>
+      </c>
+      <c r="E36" s="3">
+        <v>57.723300000000002</v>
+      </c>
+      <c r="F36" s="3">
+        <v>-1.2223900000000001</v>
+      </c>
+      <c r="G36" s="3">
+        <v>2.4043100000000002</v>
+      </c>
+      <c r="H36" s="3">
+        <v>45.359200000000001</v>
+      </c>
+      <c r="I36" s="3">
+        <v>7.2449099999999996E-4</v>
+      </c>
+      <c r="J36" s="3">
+        <v>-1.2175E-3</v>
+      </c>
+      <c r="K36" s="3">
+        <v>26.45</v>
+      </c>
+      <c r="L36" s="3">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="M36" s="3">
+        <v>16.649999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2.0231300000000001</v>
+      </c>
+      <c r="C39" s="3">
+        <v>-33.007899999999999</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.29850500000000002</v>
+      </c>
+      <c r="E39" s="3">
+        <v>66.3583</v>
+      </c>
+      <c r="F39" s="3">
+        <v>-0.94679800000000003</v>
+      </c>
+      <c r="G39" s="3">
+        <v>-3.1187</v>
+      </c>
+      <c r="H39" s="3">
+        <v>38.234299999999998</v>
+      </c>
+      <c r="I39" s="3">
+        <v>8.3561699999999998E-4</v>
+      </c>
+      <c r="J39" s="3">
+        <v>-4.0543300000000002E-4</v>
+      </c>
+      <c r="K39" s="3">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="L39" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="M39" s="3">
+        <v>20.55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3">
+        <v>-12.3085</v>
+      </c>
+      <c r="C42" s="3">
+        <v>-51.578000000000003</v>
+      </c>
+      <c r="D42" s="3">
+        <v>3.30951</v>
+      </c>
+      <c r="E42" s="3">
+        <v>51.435499999999998</v>
+      </c>
+      <c r="F42" s="3">
+        <v>7.9262399999999993E-3</v>
+      </c>
+      <c r="G42" s="3">
+        <v>3.8865400000000001</v>
+      </c>
+      <c r="H42" s="3">
+        <v>51.905000000000001</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1.2945299999999999E-3</v>
+      </c>
+      <c r="J42" s="3">
+        <v>-7.8853899999999999E-4</v>
+      </c>
+      <c r="K42" s="3">
+        <v>21</v>
+      </c>
+      <c r="L42" s="3">
+        <v>22.35</v>
+      </c>
+      <c r="M42" s="3">
+        <v>26.85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <f>MIN(B2:B51)</f>
+        <v>-31.913699999999999</v>
+      </c>
+      <c r="C53" s="4">
+        <f t="shared" ref="C53:M53" si="0">MIN(C2:C51)</f>
+        <v>-68.405299999999997</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.2433100000000001</v>
+      </c>
+      <c r="E53" s="4">
+        <f t="shared" si="0"/>
+        <v>22.186</v>
+      </c>
+      <c r="F53" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.3935399999999998</v>
+      </c>
+      <c r="G53" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.9581799999999996</v>
+      </c>
+      <c r="H53" s="4">
+        <f t="shared" si="0"/>
+        <v>26.925799999999999</v>
+      </c>
+      <c r="I53" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.59472E-4</v>
+      </c>
+      <c r="J53" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.4708600000000001E-3</v>
+      </c>
+      <c r="K53" s="4">
+        <f t="shared" si="0"/>
+        <v>3.55</v>
+      </c>
+      <c r="L53" s="4">
+        <f t="shared" si="0"/>
+        <v>4.7</v>
+      </c>
+      <c r="M53" s="4">
+        <f t="shared" si="0"/>
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="4">
+        <f>MAX(B2:B51)</f>
+        <v>2.5850900000000001</v>
+      </c>
+      <c r="C54" s="4">
+        <f t="shared" ref="C54:M54" si="1">MAX(C2:C51)</f>
+        <v>-18.628</v>
+      </c>
+      <c r="D54" s="4">
+        <f t="shared" si="1"/>
+        <v>5.1007199999999999</v>
+      </c>
+      <c r="E54" s="4">
+        <f t="shared" si="1"/>
+        <v>85.751999999999995</v>
+      </c>
+      <c r="F54" s="4">
+        <f t="shared" si="1"/>
+        <v>6.4812500000000002</v>
+      </c>
+      <c r="G54" s="4">
+        <f t="shared" si="1"/>
+        <v>13.545999999999999</v>
+      </c>
+      <c r="H54" s="4">
+        <f t="shared" si="1"/>
+        <v>127.508</v>
+      </c>
+      <c r="I54" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8503E-3</v>
+      </c>
+      <c r="J54" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="4">
+        <f t="shared" si="1"/>
+        <v>34.950000000000003</v>
+      </c>
+      <c r="L54" s="4">
+        <f t="shared" si="1"/>
+        <v>35.950000000000003</v>
+      </c>
+      <c r="M54" s="4">
+        <f t="shared" si="1"/>
+        <v>43.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove unused variable from Grammar
</commit_message>
<xml_diff>
--- a/parameter_estimation.xlsx
+++ b/parameter_estimation.xlsx
@@ -468,7 +468,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,48 +1020,48 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>-11.6493</v>
+        <v>-11.703900000000001</v>
       </c>
       <c r="C12" s="3">
-        <v>-44.519199999999998</v>
+        <v>-44.525700000000001</v>
       </c>
       <c r="D12" s="3">
-        <v>-1.6929000000000001</v>
+        <v>-1.6928000000000001</v>
       </c>
       <c r="E12" s="3">
-        <v>81.7029</v>
+        <v>81.712800000000001</v>
       </c>
       <c r="F12" s="3">
-        <v>4.3493500000000003</v>
+        <v>4.5108499999999996</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>0.15044292172685861</v>
+        <v>0.1560566956810539</v>
       </c>
       <c r="H12" s="3">
-        <v>-1.2929299999999999</v>
+        <v>-1.22776</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="1"/>
-        <v>-4.4722123257109059E-2</v>
+        <v>-4.2475402349750217E-2</v>
       </c>
       <c r="J12" s="3">
-        <v>28.910299999999999</v>
+        <v>28.905200000000001</v>
       </c>
       <c r="K12" s="3">
-        <v>-6.0026200000000002E-2</v>
+        <v>-6.0315899999999999E-2</v>
       </c>
       <c r="L12" s="3">
-        <v>-0.31421700000000002</v>
+        <v>-0.31311099999999997</v>
       </c>
       <c r="M12" s="3">
-        <v>15.5</v>
+        <v>15.27</v>
       </c>
       <c r="N12" s="3">
         <v>12.8</v>
       </c>
       <c r="O12" s="3">
-        <v>35.75</v>
+        <v>35.97</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="J53" s="4">
         <f t="shared" si="2"/>
-        <v>28.910299999999999</v>
+        <v>28.905200000000001</v>
       </c>
       <c r="K53" s="4">
         <f t="shared" si="2"/>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="E54" s="4">
         <f t="shared" si="4"/>
-        <v>81.7029</v>
+        <v>81.712800000000001</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Fix a bug in VanishingPointPM
</commit_message>
<xml_diff>
--- a/parameter_estimation.xlsx
+++ b/parameter_estimation.xlsx
@@ -466,9 +466,9 @@
   </sheetPr>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,13 +859,13 @@
         <v>-5.3522800000000001E-3</v>
       </c>
       <c r="M8" s="3">
-        <v>13.75</v>
+        <v>13.752000000000001</v>
       </c>
       <c r="N8" s="3">
-        <v>8.9499999999999993</v>
+        <v>9.1519999999999992</v>
       </c>
       <c r="O8" s="3">
-        <v>46.2</v>
+        <v>46.32</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1412,48 +1412,48 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>-14.326700000000001</v>
+        <v>-14.7011</v>
       </c>
       <c r="C20" s="3">
-        <v>-42.782699999999998</v>
+        <v>-42.977499999999999</v>
       </c>
       <c r="D20" s="3">
-        <v>0.58668299999999995</v>
+        <v>0.58750899999999995</v>
       </c>
       <c r="E20" s="3">
-        <v>64.107799999999997</v>
+        <v>64.171000000000006</v>
       </c>
       <c r="F20" s="3">
-        <v>-1.69309</v>
+        <v>-1.97183</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="0"/>
-        <v>-4.2406975113212841E-2</v>
+        <v>-4.9388600569069852E-2</v>
       </c>
       <c r="H20" s="3">
-        <v>0.57217300000000004</v>
+        <v>0.83770800000000001</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="1"/>
-        <v>1.4331267783432855E-2</v>
+        <v>2.0982146435298363E-2</v>
       </c>
       <c r="J20" s="3">
         <v>39.924799999999998</v>
       </c>
       <c r="K20" s="3">
-        <v>3.47762E-2</v>
+        <v>2.3626600000000001E-2</v>
       </c>
       <c r="L20" s="3">
-        <v>-0.26711299999999999</v>
+        <v>-0.256492</v>
       </c>
       <c r="M20" s="3">
-        <v>29.8</v>
+        <v>29.806000000000001</v>
       </c>
       <c r="N20" s="3">
-        <v>21.65</v>
+        <v>21.664000000000001</v>
       </c>
       <c r="O20" s="3">
-        <v>18.649999999999999</v>
+        <v>18.673999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add texture mapping, and more
- add texture mapping,
- fix lines_31 in VanishingPointPM
- add CVUtils
</commit_message>
<xml_diff>
--- a/parameter_estimation.xlsx
+++ b/parameter_estimation.xlsx
@@ -467,8 +467,8 @@
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O42" sqref="O42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,13 +663,13 @@
         <v>-7.58028E-4</v>
       </c>
       <c r="M4" s="3">
-        <v>20.75</v>
+        <v>20.744</v>
       </c>
       <c r="N4" s="3">
-        <v>36.65</v>
+        <v>36.659999999999997</v>
       </c>
       <c r="O4" s="3">
-        <v>12.55</v>
+        <v>12.51</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update CGA grammars based on building photos
</commit_message>
<xml_diff>
--- a/parameter_estimation.xlsx
+++ b/parameter_estimation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>No.</t>
   </si>
@@ -77,6 +77,33 @@
   <si>
     <t>Pos Y / Pos Z</t>
   </si>
+  <si>
+    <t>roof_height=1.03</t>
+  </si>
+  <si>
+    <t>roof_overhang=1.065</t>
+  </si>
+  <si>
+    <t>roof_overhang=0.696</t>
+  </si>
+  <si>
+    <t>roof_height=0.78</t>
+  </si>
+  <si>
+    <t>roof_overhang=0.4971</t>
+  </si>
+  <si>
+    <t>roof_height=0.6365</t>
+  </si>
+  <si>
+    <t>roof_overhang=0.810297</t>
+  </si>
+  <si>
+    <t>roof_overhang=0.8648</t>
+  </si>
+  <si>
+    <t>roof_slope=21.5</t>
+  </si>
 </sst>
 </file>
 
@@ -119,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -142,11 +169,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -157,6 +195,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,11 +503,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,9 +515,10 @@
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -574,7 +614,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -623,7 +663,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -671,8 +711,14 @@
       <c r="O4" s="3">
         <v>12.51</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -721,7 +767,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -770,7 +816,7 @@
         <v>16.006</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -819,7 +865,7 @@
         <v>13.45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -868,7 +914,7 @@
         <v>46.32</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -916,8 +962,14 @@
       <c r="O9" s="3">
         <v>15.224</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -966,7 +1018,7 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1015,7 +1067,7 @@
         <v>11.912000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1064,7 +1116,7 @@
         <v>35.97</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1113,7 +1165,7 @@
         <v>18.850000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1162,7 +1214,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1210,8 +1262,14 @@
       <c r="O15" s="3">
         <v>17.891999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2047,7 +2105,7 @@
         <v>32.06</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2099,7 +2157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2148,7 +2206,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2197,7 +2255,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2246,7 +2304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2298,7 +2356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2350,7 +2408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2399,7 +2457,7 @@
         <v>45.169899999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2451,7 +2509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2500,7 +2558,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2548,8 +2606,14 @@
       <c r="O42" s="3">
         <v>27.597899999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2598,7 +2662,7 @@
         <v>23.35</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2646,8 +2710,14 @@
       <c r="O44" s="3">
         <v>28.011900000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2696,7 +2766,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2745,7 +2815,7 @@
         <v>23.917899999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2794,7 +2864,7 @@
         <v>21.893999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>

</xml_diff>